<commit_message>
cambios - correcciones leonel
</commit_message>
<xml_diff>
--- a/data/PlanesEstudio/INC-1704 Gestion Financiera para Proyectos de Innovacion.xlsx
+++ b/data/PlanesEstudio/INC-1704 Gestion Financiera para Proyectos de Innovacion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alegu\Desktop\DUAL\Dual\data\PlanesEstudio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E8AEC3-00CB-497D-8974-016911F3F200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3322CF-708D-4203-A6B8-E83DFA47649F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="307" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="307" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generales" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="150">
   <si>
     <t>Nombre</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Habilidades en el uso de las tecnologias de la informacion de diversas fuentes</t>
   </si>
   <si>
-    <t>Herramientas para la innovacion Tecnologica</t>
-  </si>
-  <si>
     <t>Capacidad de analisis, sintesis, organizar tiempo y planificar</t>
   </si>
   <si>
@@ -217,24 +214,6 @@
     <t xml:space="preserve">Identifica y desarrolla habilidades que permitan comprender las necesidades del mercado para ser traducidas en un producto, proceso, formas de organización o mercadotecnia.  </t>
   </si>
   <si>
-    <t>Fundamentos de la gestion financiera</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Definición y objetivo,Curva de adopción de la tecnología vs financiamiento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nivel de madurez de la tecnología versus financiamiento, Usos del financiamiento y su importancia </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Costos fijos y costos variables,Costo de producción del producto mínimo viable </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gasto corriente, Gasto de capital, Punto de Equilibrio </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analiza los esquemas de financiamiento más  adecuados al nivel de desarrollo tecnológico y los elementos más relevantes de la inversión para la evaluar la rentabilidad de la misma. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Llevar a cabo actividades grupales que propicien la selección de propuestas tecnológicas susceptibles de ser financiadas. </t>
   </si>
   <si>
@@ -244,51 +223,21 @@
     <t>Desarrollar prácticas en las que se identifiquen los gastos corrientes y de capital necesarios para llevar a cabo la propuesta de desarrollo tecnológico.</t>
   </si>
   <si>
-    <t xml:space="preserve">Investigar la relación entre el TRL (Technology Readiness Level),  IRL (Investment Readiness Level) y modelo canvas. </t>
-  </si>
-  <si>
     <t>Fuentes de financiamiento</t>
   </si>
   <si>
-    <t>Conceptos generales, Origen del Financiamiento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Financiamiento Público, Federal, Estatal y Municipal </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Financiamiento Privado, Estructura de capital,Estrategia de salida, Familia y Amigos, Capital semilla (inversión vs. acciones) </t>
-  </si>
-  <si>
     <t xml:space="preserve">Capital en crecimiento </t>
   </si>
   <si>
-    <t xml:space="preserve">Oferta Pública Inicial </t>
-  </si>
-  <si>
     <t xml:space="preserve">Identifica y aplica los esquemas de financiamiento más adecuados al nivel de desarrollo tecnológico, así como los elementos más relevantes de la inversión para determinar la rentabilidad de la misma.  </t>
   </si>
   <si>
-    <t xml:space="preserve"> Buscar, seleccionar y analizar información relativa a los conceptos de las fuentes de financiamiento. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Desarrollar una estrategia de financiamiento de mediano plazo que permita financiar en el tiempo la propuesta de desarrollo tecnológico seleccionada en el tema anterior. </t>
   </si>
   <si>
     <t>Realizar una investigación de las fuentes de financiamiento público que existen en  México,  así como fuentes internacionales.</t>
   </si>
   <si>
-    <t>Realizar una investigación de los fondos de capital semilla y capital de riesgo en mexico</t>
-  </si>
-  <si>
-    <t>Finanzas para la innovacion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contabilidad vs Finanzas, Valor del dinero en el tiempo, Interés, Tasa libre de riesgo </t>
-  </si>
-  <si>
-    <t>Flujos de efectivo,Punto de equilibrio, Rentabilida</t>
-  </si>
-  <si>
     <t>VPN</t>
   </si>
   <si>
@@ -301,27 +250,9 @@
     <t xml:space="preserve">Determinar los costos fijos y variables, así como el punto de equilibrio para la propuesta presentada. </t>
   </si>
   <si>
-    <t xml:space="preserve">Desarrollar flujos de efectivo, estado de resultados, estado de situación financiera,  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Evalúa la rentabilidad de la propuesta seleccionada anteriormente y determina el valor de la compañía al término de la inversión. </t>
   </si>
   <si>
-    <t>Evacion de riesgos</t>
-  </si>
-  <si>
-    <t>Definición, Tipos de riesgo</t>
-  </si>
-  <si>
-    <t>Riesgos de mercado, Riesgo de volatilidad</t>
-  </si>
-  <si>
-    <t>Riesgo de liquidez,Riesgo sistémico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Análisis de sensibilidad,Árbol de decisiones </t>
-  </si>
-  <si>
     <t>Identifica y determina el nivel de riesgo de la propuesta tecnológica presentada para la determinación de la viabilidad financiera de la misma</t>
   </si>
   <si>
@@ -476,13 +407,97 @@
   </si>
   <si>
     <t>INC-1704T04CEO1A2</t>
+  </si>
+  <si>
+    <t>TEMA EXTRA NO VALIDA</t>
+  </si>
+  <si>
+    <t>Fundamentos de la gestión financiera</t>
+  </si>
+  <si>
+    <t>Definición y objetivo, Curva de adopción de la tecnología vs. Financiamiento</t>
+  </si>
+  <si>
+    <t>Nivel de madurez de la tecnología versus financiamiento, usos del financiamiento y su importancia</t>
+  </si>
+  <si>
+    <t>Costos fijos y costos variables, Costo de producción del producto mínimo viable</t>
+  </si>
+  <si>
+    <t>Gasto corriente, gasto de capital, punto de equilibrio</t>
+  </si>
+  <si>
+    <t>Analiza los esquemas de financiamiento más  adecuados al nivel de desarrollo tecnológico y los elementos más relevantes de la inversión para la evalúa la rentabilidad de la misma.</t>
+  </si>
+  <si>
+    <t>Capacidad de análisis, síntesis, organizar tiempo y planificar</t>
+  </si>
+  <si>
+    <t>Habilidades para la solución de problemas</t>
+  </si>
+  <si>
+    <t>Habilidad para buscar, procesar y analizar información de diversas fuentes</t>
+  </si>
+  <si>
+    <t>Habilidades en el uso de las tecnologías de la información de diversas fuentes</t>
+  </si>
+  <si>
+    <t>Compromiso ético, preservación del ambiente e identificar plantear y resolver problemas, liderazgo y creatividad</t>
+  </si>
+  <si>
+    <t>Investigar la relación entre el TRL (Technology Readiness Level),  IRL (Investment Readiness Level) y modelo canvas.</t>
+  </si>
+  <si>
+    <t>Conceptos generales, origen del financiamiento</t>
+  </si>
+  <si>
+    <t>Financiamiento público, federal, estatal y municipal</t>
+  </si>
+  <si>
+    <t>Financiamiento privado, estructura de Capital, estrategia de Salida, familia y amigos, capital semilla (inversión vs. acciones)</t>
+  </si>
+  <si>
+    <t>Oferta pública inicial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscar, seleccionar y analizar información relativa a los conceptos de las fuentes de financiamiento. </t>
+  </si>
+  <si>
+    <t>Realizar una investigación de los fondos de capital, semilla y capital de riesgo en México</t>
+  </si>
+  <si>
+    <t>Finanzas para la innovación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contabilidad vs. finanzas, valor del Dinero en el Tiempo, interés, tasa libre de riesgo </t>
+  </si>
+  <si>
+    <t>Flujos de efectivo, punto de equilibrio, Rentabilidad</t>
+  </si>
+  <si>
+    <t>Desarrollar flujos de efectivo, estado de resultados, estado de situación financiera</t>
+  </si>
+  <si>
+    <t>Evasión de riesgos</t>
+  </si>
+  <si>
+    <t>Definición, tipos de riesgo</t>
+  </si>
+  <si>
+    <t>Riesgos de mercado, riesgo de volatilidad</t>
+  </si>
+  <si>
+    <t>Riesgo de liquidez, Riesgo sistémico</t>
+  </si>
+  <si>
+    <t>Análisis de sensibilidad, Árbol de decisiones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -512,9 +527,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -664,7 +694,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -744,6 +774,58 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1077,7 +1159,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1090,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1164,7 +1246,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1175,7 +1257,7 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1186,7 +1268,7 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1197,7 +1279,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1228,7 +1310,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1239,7 +1321,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1250,7 +1332,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1261,7 +1343,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1272,7 +1354,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1559,8 +1641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView topLeftCell="C29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1592,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="6"/>
@@ -1688,10 +1770,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>59</v>
+        <v>124</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="1"/>
@@ -1706,10 +1788,10 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="8" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>60</v>
+        <v>125</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="1"/>
@@ -1724,10 +1806,10 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="8" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>61</v>
+        <v>126</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="1"/>
@@ -1742,10 +1824,10 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="8" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="1"/>
@@ -1874,10 +1956,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>63</v>
+        <v>128</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1959,10 +2041,10 @@
         <v>5</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="1"/>
@@ -1977,10 +2059,10 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="8" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>18</v>
+        <v>130</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="1"/>
@@ -1995,10 +2077,10 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="8" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>19</v>
+        <v>131</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="1"/>
@@ -2013,10 +2095,10 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="8" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>20</v>
+        <v>132</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="1"/>
@@ -2031,10 +2113,10 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="8" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>23</v>
+        <v>133</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="1"/>
@@ -2135,10 +2217,10 @@
         <v>4</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E37" s="11">
         <v>0.5</v>
@@ -2162,10 +2244,10 @@
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="8" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E38" s="12">
         <v>1</v>
@@ -2189,10 +2271,10 @@
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="8" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E39" s="11">
         <v>0.5</v>
@@ -2216,10 +2298,10 @@
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="8" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>67</v>
+        <v>134</v>
       </c>
       <c r="E40" s="11">
         <v>0.5</v>
@@ -2606,8 +2688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView topLeftCell="D25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2633,13 +2715,13 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>68</v>
+      <c r="C2" s="27" t="s">
+        <v>60</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="6"/>
@@ -2735,10 +2817,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>69</v>
+        <v>135</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="1"/>
@@ -2753,10 +2835,10 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="8" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>70</v>
+        <v>136</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="1"/>
@@ -2771,10 +2853,10 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="8" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>71</v>
+        <v>137</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="1"/>
@@ -2789,10 +2871,10 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="8" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="1"/>
@@ -2807,10 +2889,10 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="8" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>73</v>
+        <v>138</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="1"/>
@@ -2925,10 +3007,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -3010,10 +3092,10 @@
         <v>5</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="1"/>
@@ -3028,10 +3110,10 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="8" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>18</v>
+        <v>130</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="1"/>
@@ -3046,10 +3128,10 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="8" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>19</v>
+        <v>131</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="1"/>
@@ -3064,10 +3146,10 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="8" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>20</v>
+        <v>132</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="1"/>
@@ -3082,10 +3164,10 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="8" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>23</v>
+        <v>133</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="1"/>
@@ -3186,10 +3268,10 @@
         <v>4</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>75</v>
+        <v>139</v>
       </c>
       <c r="E37" s="11">
         <v>0.5</v>
@@ -3213,10 +3295,10 @@
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="8" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="E38" s="12">
         <v>0.5</v>
@@ -3240,10 +3322,10 @@
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="8" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="E39" s="11">
         <v>0.5</v>
@@ -3267,10 +3349,10 @@
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="8" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>78</v>
+        <v>140</v>
       </c>
       <c r="E40" s="12">
         <v>0.5</v>
@@ -3657,8 +3739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView topLeftCell="B20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="D26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3690,7 +3772,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>79</v>
+        <v>141</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="6"/>
@@ -3786,10 +3868,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="1"/>
@@ -3804,10 +3886,10 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="8" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="1"/>
@@ -3822,10 +3904,10 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="8" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="1"/>
@@ -3840,10 +3922,10 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="8" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="1"/>
@@ -3972,10 +4054,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -4057,10 +4139,10 @@
         <v>5</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="1"/>
@@ -4075,10 +4157,10 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="8" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>18</v>
+        <v>130</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="1"/>
@@ -4093,10 +4175,10 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="8" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>19</v>
+        <v>131</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="1"/>
@@ -4111,10 +4193,10 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="8" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>20</v>
+        <v>132</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="1"/>
@@ -4129,10 +4211,10 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="8" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>23</v>
+        <v>133</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="1"/>
@@ -4233,10 +4315,10 @@
         <v>4</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="E37" s="11">
         <v>0.5</v>
@@ -4260,10 +4342,10 @@
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="8" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>86</v>
+        <v>144</v>
       </c>
       <c r="E38" s="12">
         <v>1</v>
@@ -4287,10 +4369,10 @@
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="8" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="E39" s="11">
         <v>0.5</v>
@@ -4692,8 +4774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="D21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4725,7 +4807,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>88</v>
+        <v>145</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="6"/>
@@ -4821,10 +4903,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>89</v>
+        <v>146</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="1"/>
@@ -4839,10 +4921,10 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="8" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="1"/>
@@ -4857,10 +4939,10 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="8" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>91</v>
+        <v>148</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="1"/>
@@ -4875,10 +4957,10 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="8" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>92</v>
+        <v>149</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="1"/>
@@ -5007,10 +5089,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -5092,10 +5174,10 @@
         <v>5</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="1"/>
@@ -5110,10 +5192,10 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="8" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>18</v>
+        <v>130</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="1"/>
@@ -5128,10 +5210,10 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="8" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>19</v>
+        <v>131</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="1"/>
@@ -5146,10 +5228,10 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="8" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>20</v>
+        <v>132</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="1"/>
@@ -5164,10 +5246,10 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D30" s="24" t="s">
-        <v>23</v>
+        <v>119</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>133</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="1"/>
@@ -5268,10 +5350,10 @@
         <v>4</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="E37" s="11">
         <v>1</v>
@@ -5295,10 +5377,10 @@
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="8" t="s">
-        <v>144</v>
+        <v>121</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="E38" s="12">
         <v>1</v>
@@ -5716,7 +5798,7 @@
   <dimension ref="A1:M65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5729,856 +5811,856 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="A1" s="32"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="32"/>
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="C2" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="32"/>
+      <c r="B4" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="36">
         <v>1</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="32"/>
+      <c r="B6" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="37">
         <v>3</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="32"/>
+      <c r="B8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="C8" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="33"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="33"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="33"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="33"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2" t="s">
+      <c r="A20" s="32"/>
+      <c r="B20" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="C20" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2" t="s">
+      <c r="A26" s="32"/>
+      <c r="B26" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
+      <c r="C26" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="33"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="24" t="s">
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="24" t="s">
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="24" t="s">
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="33"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
+      <c r="A34" s="32"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
+      <c r="A35" s="32"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
+      <c r="A36" s="32"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
     <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="2" t="s">
+      <c r="A37" s="32"/>
+      <c r="B37" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="E37" s="11">
+      <c r="C37" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="48">
         <v>0.5</v>
       </c>
-      <c r="F37" s="18" t="s">
+      <c r="F37" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="G37" s="18" t="s">
+      <c r="G37" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="H37" s="7">
+      <c r="H37" s="38">
         <v>4</v>
       </c>
-      <c r="I37" s="1"/>
+      <c r="I37" s="32"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
     </row>
     <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="E38" s="11">
+      <c r="A38" s="32"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" s="48">
         <v>0.5</v>
       </c>
-      <c r="F38" s="19" t="s">
+      <c r="F38" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="G38" s="19" t="s">
+      <c r="G38" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="H38" s="8">
+      <c r="H38" s="40">
         <v>4</v>
       </c>
-      <c r="I38" s="1"/>
+      <c r="I38" s="32"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D39" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="E39" s="11">
+      <c r="A39" s="32"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="48">
         <v>0.5</v>
       </c>
-      <c r="F39" s="19" t="s">
+      <c r="F39" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="G39" s="19" t="s">
+      <c r="G39" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="H39" s="8">
+      <c r="H39" s="40">
         <v>4</v>
       </c>
-      <c r="I39" s="1"/>
+      <c r="I39" s="32"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="E40" s="11">
+      <c r="A40" s="32"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" s="48">
         <v>0.5</v>
       </c>
-      <c r="F40" s="19" t="s">
+      <c r="F40" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="G40" s="19" t="s">
+      <c r="G40" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="H40" s="8">
+      <c r="H40" s="40">
         <v>4</v>
       </c>
-      <c r="I40" s="1"/>
+      <c r="I40" s="32"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="1"/>
+      <c r="A41" s="32"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="40"/>
+      <c r="I41" s="32"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="1"/>
+      <c r="A42" s="32"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="41"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="32"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="1"/>
+      <c r="A43" s="32"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="50"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="32"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="1"/>
+      <c r="A44" s="32"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="32"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="1"/>
+      <c r="A45" s="32"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="32"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="1"/>
+      <c r="A46" s="32"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="53"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="46"/>
+      <c r="I46" s="32"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
+      <c r="A47" s="32"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="54"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="32"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
+      <c r="A48" s="32"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="32"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
+      <c r="A49" s="32"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
+      <c r="A50" s="32"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="32"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
+      <c r="A51" s="32"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
+      <c r="A52" s="32"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="33"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
+      <c r="A53" s="32"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="32"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="32"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
@@ -6768,6 +6850,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010066362C18D9728B45B978E0202B482283" ma:contentTypeVersion="6" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="cc541c24bb563767f1b173ccc5d750be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bbe4718c-7bcc-499a-b45a-2c898923f758" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e9100314d28dd3083d9f7fd26077858e" ns2:_="">
     <xsd:import namespace="bbe4718c-7bcc-499a-b45a-2c898923f758"/>
@@ -6925,12 +7013,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{194C63B9-6D56-41B8-852C-30E254E0B949}">
   <ds:schemaRefs>
@@ -6940,6 +7022,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6484B29-A119-444E-B32B-DDD7B740B41D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bbe4718c-7bcc-499a-b45a-2c898923f758"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{683EB964-DBA5-4BF7-8665-4ABAC26A7728}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6955,20 +7053,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6484B29-A119-444E-B32B-DDD7B740B41D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bbe4718c-7bcc-499a-b45a-2c898923f758"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>